<commit_message>
updated testcase with DD
</commit_message>
<xml_diff>
--- a/TestData/search.xlsx
+++ b/TestData/search.xlsx
@@ -28,10 +28,10 @@
     <t xml:space="preserve">Saturn</t>
   </si>
   <si>
-    <t xml:space="preserve">Saturday’s Market</t>
-  </si>
-  <si>
     <t xml:space="preserve">Krux</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Saturday's Market</t>
   </si>
 </sst>
 </file>
@@ -201,7 +201,7 @@
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>